<commit_message>
Changed C8 value in BOM
</commit_message>
<xml_diff>
--- a/WBOOS v1.2/DStage_WBOOS_v1.2_BOM.xlsx
+++ b/WBOOS v1.2/DStage_WBOOS_v1.2_BOM.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="83">
   <si>
     <t>Comment</t>
   </si>
@@ -28,7 +28,7 @@
     <t>100n</t>
   </si>
   <si>
-    <t>C5, C8, C11, C12, C17</t>
+    <t>C5, C11, C12, C17</t>
   </si>
   <si>
     <t>C0805</t>
@@ -46,10 +46,13 @@
     <t>C28323</t>
   </si>
   <si>
-    <t>DNP</t>
-  </si>
-  <si>
-    <t>C7</t>
+    <t>10n</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>C1710</t>
   </si>
   <si>
     <t>1n</t>
@@ -349,20 +352,20 @@
     <xf borderId="1" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="2" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -703,374 +706,376 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="9"/>
+      <c r="D4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="8"/>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="B5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="9"/>
+        <v>16</v>
+      </c>
+      <c r="E5" s="8"/>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="B6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="B7" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="9"/>
+        <v>22</v>
+      </c>
+      <c r="E7" s="8"/>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="10"/>
+        <v>25</v>
+      </c>
+      <c r="E8" s="11"/>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="B9" s="9" t="s">
         <v>27</v>
       </c>
+      <c r="C9" s="10" t="s">
+        <v>28</v>
+      </c>
       <c r="D9" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="10"/>
+        <v>32</v>
+      </c>
+      <c r="E10" s="11"/>
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="B11" s="9" t="s">
         <v>34</v>
       </c>
+      <c r="C11" s="10" t="s">
+        <v>35</v>
+      </c>
       <c r="D11" s="4"/>
-      <c r="E11" s="10"/>
+      <c r="E11" s="11"/>
     </row>
     <row r="12">
       <c r="A12" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D12" s="4"/>
-      <c r="E12" s="9"/>
+      <c r="E12" s="8"/>
     </row>
     <row r="13">
       <c r="A13" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>39</v>
       </c>
+      <c r="C13" s="10" t="s">
+        <v>40</v>
+      </c>
       <c r="D13" s="4"/>
-      <c r="E13" s="9"/>
+      <c r="E13" s="8"/>
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" s="9"/>
+        <v>44</v>
+      </c>
+      <c r="E14" s="8"/>
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" s="7" t="s">
         <v>45</v>
       </c>
+      <c r="B15" s="9" t="s">
+        <v>46</v>
+      </c>
       <c r="C15" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E15" s="9"/>
+        <v>48</v>
+      </c>
+      <c r="E15" s="8"/>
     </row>
     <row r="16">
       <c r="A16" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E16" s="9"/>
+        <v>51</v>
+      </c>
+      <c r="E16" s="8"/>
     </row>
     <row r="17">
       <c r="A17" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B17" s="7" t="s">
         <v>52</v>
       </c>
+      <c r="B17" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="C17" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" s="9"/>
+        <v>54</v>
+      </c>
+      <c r="E17" s="8"/>
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" s="9"/>
+        <v>57</v>
+      </c>
+      <c r="E18" s="8"/>
     </row>
     <row r="19">
       <c r="A19" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" s="9"/>
+        <v>60</v>
+      </c>
+      <c r="E19" s="8"/>
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B20" s="7" t="s">
         <v>61</v>
       </c>
+      <c r="B20" s="9" t="s">
+        <v>62</v>
+      </c>
       <c r="C20" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E20" s="9"/>
+        <v>63</v>
+      </c>
+      <c r="E20" s="8"/>
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C21" s="8" t="s">
         <v>65</v>
       </c>
+      <c r="C21" s="10" t="s">
+        <v>66</v>
+      </c>
       <c r="D21" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E21" s="9"/>
+        <v>67</v>
+      </c>
+      <c r="E21" s="8"/>
     </row>
     <row r="22">
-      <c r="A22" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B22" s="7" t="s">
+      <c r="A22" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="B22" s="9" t="s">
         <v>69</v>
       </c>
+      <c r="C22" s="10" t="s">
+        <v>70</v>
+      </c>
       <c r="D22" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E22" s="9"/>
+        <v>71</v>
+      </c>
+      <c r="E22" s="8"/>
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E23" s="10"/>
+        <v>75</v>
+      </c>
+      <c r="E23" s="11"/>
     </row>
     <row r="24">
-      <c r="A24" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B24" s="7" t="s">
+      <c r="A24" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="B24" s="9" t="s">
         <v>77</v>
       </c>
+      <c r="C24" s="10" t="s">
+        <v>78</v>
+      </c>
       <c r="D24" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E24" s="10"/>
+        <v>79</v>
+      </c>
+      <c r="E24" s="11"/>
     </row>
     <row r="25">
-      <c r="A25" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="B25" s="7" t="s">
+      <c r="A25" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>65</v>
+      <c r="B25" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>66</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E25" s="9"/>
+        <v>82</v>
+      </c>
+      <c r="E25" s="8"/>
     </row>
     <row r="26">
-      <c r="E26" s="9"/>
+      <c r="E26" s="8"/>
     </row>
     <row r="27">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="6"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="9"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="8"/>
     </row>
     <row r="28">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="8"/>
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="10"/>
       <c r="D28" s="12"/>
-      <c r="E28" s="9"/>
+      <c r="E28" s="8"/>
     </row>
     <row r="29">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="6"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="9"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="8"/>
     </row>
     <row r="30">
       <c r="A30" s="13"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="8"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="10"/>
       <c r="D30" s="12"/>
-      <c r="E30" s="10"/>
+      <c r="E30" s="11"/>
     </row>
     <row r="31">
       <c r="A31" s="14"/>
       <c r="B31" s="5"/>
       <c r="C31" s="6"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="9"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="8"/>
     </row>
     <row r="32">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="8"/>
+      <c r="A32" s="9"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="10"/>
       <c r="D32" s="12"/>
     </row>
     <row r="33">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="6"/>
-      <c r="D33" s="11"/>
+      <c r="D33" s="7"/>
     </row>
     <row r="34">
       <c r="A34" s="15"/>

</xml_diff>